<commit_message>
Altera especificação após reunição com a SEF
</commit_message>
<xml_diff>
--- a/espec011_valor_pago/static/formulario_detalhamento_despesa.xlsx
+++ b/espec011_valor_pago/static/formulario_detalhamento_despesa.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m11483500\Documents\GitHub\especificacoes-portal-transparencia\espec011_valor_pago\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m13368964\Documents\Documents\1.CGE\Projetos-Transparencia-Ativa\especificacoes-portal-transparencia\espec011_valor_pago\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Código do Documento</t>
   </si>
@@ -38,16 +38,22 @@
     <t>29979036000140 - INSS - INSTITUTO NACIONAL DE SEGURIDADE SOCIAL</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Pagamento</t>
   </si>
   <si>
     <t>Data Registro</t>
   </si>
   <si>
-    <t>Data Pagamento</t>
+    <t>Situação da Ordem de Pagamento</t>
+  </si>
+  <si>
+    <t>Pedente de Transmissão aos bancos</t>
+  </si>
+  <si>
+    <t>Acatada pelo Banco</t>
+  </si>
+  <si>
+    <t>Sujeita a compesação bancária</t>
   </si>
 </sst>
 </file>
@@ -162,9 +168,6 @@
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -176,6 +179,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -460,39 +466,39 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="79.28515625" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -506,10 +512,10 @@
       <c r="B4" s="2">
         <v>43797</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="1">
@@ -523,10 +529,10 @@
       <c r="B5" s="2">
         <v>43797</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="1">
@@ -540,10 +546,10 @@
       <c r="B6" s="2">
         <v>43797</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="1">

</xml_diff>